<commit_message>
Working Checkpoint. Reading String from Template and Replacing Chars for Body
</commit_message>
<xml_diff>
--- a/recruiters.xlsx
+++ b/recruiters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danis/Git/emailRecruit/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Company</t>
   </si>
@@ -38,17 +35,67 @@
     <t>Mail ID</t>
   </si>
   <si>
-    <t>Position</t>
+    <t>NC State</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>ghi</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>def@gmail.com</t>
+  </si>
+  <si>
+    <t>ghi@gmail.com</t>
+  </si>
+  <si>
+    <t>Position Applying For</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>abc Engineer</t>
+  </si>
+  <si>
+    <t>def Engineer</t>
+  </si>
+  <si>
+    <t>ghi Engineer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,13 +118,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -353,29 +403,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working Checkpoint. Read and Parse from Excel
</commit_message>
<xml_diff>
--- a/recruiters.xlsx
+++ b/recruiters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Company</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>ghi Engineer</t>
+  </si>
+  <si>
+    <t>Job ID</t>
   </si>
 </sst>
 </file>
@@ -403,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -415,7 +418,7 @@
     <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -431,8 +434,11 @@
       <c r="E1" t="s">
         <v>11</v>
       </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -446,7 +452,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -460,7 +466,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>